<commit_message>
update all nomis datasets (with correct LSIPs) and reload update ilr dataset and reload update data table with latest dates and next releases
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\3-1_DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2860D04-B9BE-4882-B709-F6C7125360C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C78FD9-0072-45AD-800C-2B85D8C1B606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>Data​</t>
   </si>
@@ -53,9 +53,6 @@
     <t>&lt;a href='https://www.nomisweb.co.uk/datasets/apsnew'&gt;Annual Population Survey&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Oct 2021 - Sep 2022 (17/01/23)</t>
-  </si>
-  <si>
     <t>To be announced</t>
   </si>
   <si>
@@ -65,9 +62,6 @@
     <t>Jan 2021 - Dec 2021 (12/04/22)</t>
   </si>
   <si>
-    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/further-education-and-skills/2021-22'&gt;Individualised Learner Record&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Aug 2021 – Jul 2022 (24/11/22)</t>
   </si>
   <si>
@@ -159,6 +153,27 @@
   </si>
   <si>
     <t>Aug 2022 – Jul 2023 (Nov 23)</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/further-education-and-skills/2022-23'&gt;Individualised Learner Record&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Aug 2021 – Jul 2022 (31/03/23)</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.nomisweb.co.uk/livelinks/16244.xlsx'&gt;Annual Population Survey&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.nomisweb.co.uk/livelinks/16243.xlsx'&gt;Annual Population Survey&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.nomisweb.co.uk/livelinks/16246.xlsx'&gt;ONS UK Business Counts&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>TBC</t>
+  </si>
+  <si>
+    <t>Apr 2022 - Mar 2023 (11/06/23)</t>
   </si>
 </sst>
 </file>
@@ -545,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -572,184 +587,184 @@
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>5</v>
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
         <v>33</v>
       </c>
-      <c r="B14" t="s">
-        <v>35</v>
-      </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tidy code ignore ilr partial year calculate for entreprise and use dorset lep for dorset lsip add note to local skills page about the issue updated updated data notes for the issue updated data page for the issue
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\3-1_DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C78FD9-0072-45AD-800C-2B85D8C1B606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C330184-E784-4036-AC60-C05B5A211A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>Data​</t>
   </si>
@@ -170,10 +170,13 @@
     <t>&lt;a href='https://www.nomisweb.co.uk/livelinks/16246.xlsx'&gt;ONS UK Business Counts&lt;/a&gt;</t>
   </si>
   <si>
-    <t>TBC</t>
-  </si>
-  <si>
     <t>Apr 2022 - Mar 2023 (11/06/23)</t>
+  </si>
+  <si>
+    <t>TBC depending on ONS resolving the SOC coding issue</t>
+  </si>
+  <si>
+    <t>TBC depending on ONS recoding the qualification framework.</t>
   </si>
 </sst>
 </file>
@@ -561,7 +564,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -596,7 +599,7 @@
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -610,7 +613,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -624,7 +627,7 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -666,7 +669,7 @@
         <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added note that a direct download. Added note about partial year
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\3-1_DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C330184-E784-4036-AC60-C05B5A211A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EC2F3D-0579-4D6A-979D-A968ADC9AB27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="20" yWindow="600" windowWidth="22540" windowHeight="14440" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -161,12 +161,6 @@
     <t>Aug 2021 – Jul 2022 (31/03/23)</t>
   </si>
   <si>
-    <t>&lt;a href='https://www.nomisweb.co.uk/livelinks/16244.xlsx'&gt;Annual Population Survey&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://www.nomisweb.co.uk/livelinks/16243.xlsx'&gt;Annual Population Survey&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>&lt;a href='https://www.nomisweb.co.uk/livelinks/16246.xlsx'&gt;ONS UK Business Counts&lt;/a&gt;</t>
   </si>
   <si>
@@ -177,6 +171,12 @@
   </si>
   <si>
     <t>TBC depending on ONS recoding the qualification framework.</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.nomisweb.co.uk/livelinks/16244.xlsx'&gt;Annual Population Survey (direct download)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.nomisweb.co.uk/livelinks/16243.xlsx'&gt;Annual Population Survey (direct download)&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -564,7 +564,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -593,13 +593,13 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -613,7 +613,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -621,13 +621,13 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -669,7 +669,7 @@
         <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -677,7 +677,7 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Update date of aps next update
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\3-1_DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EC2F3D-0579-4D6A-979D-A968ADC9AB27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="600" windowWidth="22540" windowHeight="14440" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -164,9 +164,6 @@
     <t>&lt;a href='https://www.nomisweb.co.uk/livelinks/16246.xlsx'&gt;ONS UK Business Counts&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Apr 2022 - Mar 2023 (11/06/23)</t>
-  </si>
-  <si>
     <t>TBC depending on ONS resolving the SOC coding issue</t>
   </si>
   <si>
@@ -177,6 +174,9 @@
   </si>
   <si>
     <t>&lt;a href='https://www.nomisweb.co.uk/livelinks/16243.xlsx'&gt;Annual Population Survey (direct download)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Apr 2022 - Mar 2023 (11/07/23)</t>
   </si>
 </sst>
 </file>
@@ -564,7 +564,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -593,13 +593,13 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -613,7 +613,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -621,13 +621,13 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -669,7 +669,7 @@
         <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update with soc2020 add local market profile to tools list Change date of punblivcaion
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\3-1_DataTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36A67C19-DECB-4C24-B62E-0E2BB0634240}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>Data​</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Further education and skills achievements by sector subject area</t>
   </si>
   <si>
-    <t>Jan 2021 - Dec 2021 (12/04/22)</t>
-  </si>
-  <si>
     <t>Aug 2021 – Jul 2022 (24/11/22)</t>
   </si>
   <si>
@@ -164,9 +161,6 @@
     <t>&lt;a href='https://www.nomisweb.co.uk/livelinks/16246.xlsx'&gt;ONS UK Business Counts&lt;/a&gt;</t>
   </si>
   <si>
-    <t>TBC depending on ONS resolving the SOC coding issue</t>
-  </si>
-  <si>
     <t>TBC depending on ONS recoding the qualification framework.</t>
   </si>
   <si>
@@ -176,7 +170,10 @@
     <t>&lt;a href='https://www.nomisweb.co.uk/livelinks/16243.xlsx'&gt;Annual Population Survey (direct download)&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Apr 2022 - Mar 2023 (11/07/23)</t>
+    <t>Apr 2022 - Mar 2023 (15/08/23)</t>
+  </si>
+  <si>
+    <t>Jan 2022 - Dec 2022 (07/23)</t>
   </si>
 </sst>
 </file>
@@ -238,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
@@ -246,7 +243,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,58 +586,58 @@
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
         <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>7</v>
+      <c r="C3" t="s">
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -649,108 +645,108 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
         <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
         <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
       <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -758,13 +754,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
         <v>31</v>
-      </c>
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" t="s">
-        <v>32</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
update to latest nomis data make correction to some of the lep names
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36A67C19-DECB-4C24-B62E-0E2BB0634240}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{774D4C53-4EF7-4013-9F86-748BD81FFF31}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>Data​</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Jan 2021 - Dec 2021 (20/04/22)</t>
   </si>
   <si>
-    <t>Jan 2022 - Dec 2022 (19/04/23)</t>
-  </si>
-  <si>
     <t>Key Stage 4 (KS4) destinations</t>
   </si>
   <si>
@@ -164,16 +161,10 @@
     <t>TBC depending on ONS recoding the qualification framework.</t>
   </si>
   <si>
-    <t>&lt;a href='https://www.nomisweb.co.uk/livelinks/16244.xlsx'&gt;Annual Population Survey (direct download)&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://www.nomisweb.co.uk/livelinks/16243.xlsx'&gt;Annual Population Survey (direct download)&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Apr 2022 - Mar 2023 (15/08/23)</t>
   </si>
   <si>
-    <t>Jan 2022 - Dec 2022 (07/23)</t>
+    <t>Jul 2022 - Jun 2023 (17/10/23)</t>
   </si>
 </sst>
 </file>
@@ -560,12 +551,12 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="174.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="86.7265625" customWidth="1"/>
     <col min="2" max="2" width="39.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.36328125" bestFit="1" customWidth="1"/>
   </cols>
@@ -586,30 +577,30 @@
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
         <v>42</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -617,27 +608,27 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -651,7 +642,7 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -665,7 +656,7 @@
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -673,7 +664,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -684,7 +675,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -712,30 +703,30 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
@@ -743,10 +734,10 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -754,13 +745,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
         <v>30</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
updtae business count data update renv
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{774D4C53-4EF7-4013-9F86-748BD81FFF31}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47A26503-18DE-452F-91AA-9A7DCDE7F944}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>Data​</t>
   </si>
@@ -65,12 +65,6 @@
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/cae2bcbb-e385-4da7-8d7b-08dacbbccc68'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Mar 2022 (28/09/22)</t>
-  </si>
-  <si>
-    <t>Mar 2023 (03/10/23)</t>
-  </si>
-  <si>
     <t>Employment by industry</t>
   </si>
   <si>
@@ -155,9 +149,6 @@
     <t>Aug 2021 – Jul 2022 (31/03/23)</t>
   </si>
   <si>
-    <t>&lt;a href='https://www.nomisweb.co.uk/livelinks/16246.xlsx'&gt;ONS UK Business Counts&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>TBC depending on ONS recoding the qualification framework.</t>
   </si>
   <si>
@@ -165,6 +156,12 @@
   </si>
   <si>
     <t>Jul 2022 - Jun 2023 (17/10/23)</t>
+  </si>
+  <si>
+    <t>Mar 2023 (27/09/23)</t>
+  </si>
+  <si>
+    <t>Mar 2024 (09/24)</t>
   </si>
 </sst>
 </file>
@@ -551,7 +548,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -577,58 +574,58 @@
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -642,102 +639,102 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -745,13 +742,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Update destinatios data to 21/22
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47A26503-18DE-452F-91AA-9A7DCDE7F944}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96E49CD0-0C79-4EB6-9226-47294B224AAE}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -101,18 +101,6 @@
     <t>Key Stage 5 (KS5) destinations</t>
   </si>
   <si>
-    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/1683bef5-5daa-49d7-9323-08db08498a11'&gt;National Pupil Database&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/1703fe2c-2e57-4bfe-9325-08db08498a11'&gt;National Pupil Database&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>Aug 2020 -  Jul 2021 (19/20 learners) (02/02/23)</t>
-  </si>
-  <si>
-    <t>Aug 2021 -  Jul 2022 (20/21 learners) (Oct 23)</t>
-  </si>
-  <si>
     <t>Dec 2022 (13/02/23)</t>
   </si>
   <si>
@@ -162,6 +150,18 @@
   </si>
   <si>
     <t>Mar 2024 (09/24)</t>
+  </si>
+  <si>
+    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/f5995891-4e9a-439d-0d58-08dbd1400c33'&gt;National Pupil Database&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Aug 2021 -  Jul 2022 (20/21 learners) (19/10/23)</t>
+  </si>
+  <si>
+    <t>Aug 2022 -  Jul 2023 (21/22 learners) (Oct 24)</t>
+  </si>
+  <si>
+    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/b0424f32-b140-44a8-a039-08dbd1466a44'&gt;National Pupil Database&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -548,7 +548,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -574,30 +574,30 @@
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -608,24 +608,24 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
         <v>30</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -639,7 +639,7 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -653,7 +653,7 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -664,24 +664,24 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -703,13 +703,13 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -717,13 +717,13 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
@@ -731,10 +731,10 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -742,13 +742,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
updated employmnet aps data
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96E49CD0-0C79-4EB6-9226-47294B224AAE}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01592995-D7E7-4D87-97CA-D93995631102}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -140,18 +140,9 @@
     <t>TBC depending on ONS recoding the qualification framework.</t>
   </si>
   <si>
-    <t>Apr 2022 - Mar 2023 (15/08/23)</t>
-  </si>
-  <si>
-    <t>Jul 2022 - Jun 2023 (17/10/23)</t>
-  </si>
-  <si>
     <t>Mar 2023 (27/09/23)</t>
   </si>
   <si>
-    <t>Mar 2024 (09/24)</t>
-  </si>
-  <si>
     <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/f5995891-4e9a-439d-0d58-08dbd1400c33'&gt;National Pupil Database&lt;/a&gt;</t>
   </si>
   <si>
@@ -162,6 +153,15 @@
   </si>
   <si>
     <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/b0424f32-b140-44a8-a039-08dbd1466a44'&gt;National Pupil Database&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Mar 2024 (Sep 24)</t>
+  </si>
+  <si>
+    <t>Oct 2022 - Sep 2023 (16/01/24)</t>
+  </si>
+  <si>
+    <t>Jul 2022 - Jun 2023 (24/10/23)</t>
   </si>
 </sst>
 </file>
@@ -548,7 +548,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -580,10 +580,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -594,10 +594,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -608,10 +608,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -664,10 +664,10 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -678,10 +678,10 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -703,13 +703,13 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -717,13 +717,13 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update ilr by ssa data
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/ross_finnie_education_gov_uk/Documents/Documents/Git Projects/Local Skills Dashboard/Data/3-1_DataTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B39CDB1B-01E0-4631-A696-9AD82C342DA8}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61F2AD73-A99A-49F6-9E5B-B1CACE507CDF}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="2970" windowWidth="29040" windowHeight="15840" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>Data​</t>
   </si>
@@ -59,12 +59,6 @@
     <t>Further education and skills achievements by sector subject area</t>
   </si>
   <si>
-    <t>Aug 2021 – Jul 2022 (24/11/22)</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/cae2bcbb-e385-4da7-8d7b-08dacbbccc68'&gt;Individualised Learner Record&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Employment by industry</t>
   </si>
   <si>
@@ -122,15 +116,9 @@
     <t>Enterprises by employment industry</t>
   </si>
   <si>
-    <t>Aug 2022 – Jul 2023 (Nov 23)</t>
-  </si>
-  <si>
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/further-education-and-skills/2022-23'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Aug 2021 – Jul 2022 (31/03/23)</t>
-  </si>
-  <si>
     <t>TBC depending on ONS recoding the qualification framework.</t>
   </si>
   <si>
@@ -162,6 +150,15 @@
   </si>
   <si>
     <t>Dec 2022 - Dec 2023 (Nov 24)</t>
+  </si>
+  <si>
+    <t>Aug 2023 – Jul 2024 (Nov 24)</t>
+  </si>
+  <si>
+    <t>Aug 2022 – Jul 2023 (30/11/23)</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/93f9aa79-9a67-48d5-e9e2-08dc0dc60f26'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -548,7 +545,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -574,58 +571,58 @@
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -633,108 +630,108 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -742,13 +739,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Updtae nomis employment data (just a rerun of the exttract and transform files) update the data table and text
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61F2AD73-A99A-49F6-9E5B-B1CACE507CDF}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{938A3197-9471-48BA-9E8A-0ECCFD6F002C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -143,9 +143,6 @@
     <t>Oct 2022 - Sep 2023 (16/01/24)</t>
   </si>
   <si>
-    <t>Jul 2022 - Jun 2023 (24/10/23)</t>
-  </si>
-  <si>
     <t>Dec 2021 - Dec 2022 (22/11/23)</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/93f9aa79-9a67-48d5-e9e2-08dc0dc60f26'&gt;Individualised Learner Record&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Jan 2023 - Dec 2023 (16/04/24)</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -577,10 +577,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -591,10 +591,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -605,10 +605,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -619,10 +619,10 @@
         <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -630,13 +630,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -689,10 +689,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
         <v>36</v>
-      </c>
-      <c r="D10" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
updated to the new soc job ads data. had to do quite a lot of fiddling because the data shape had changed slightly. had to fix a correction in manchester mca where the data columns had been offset also fixed an issue with double counting in the las where a newer la exists
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{938A3197-9471-48BA-9E8A-0ECCFD6F002C}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5CCD392-972B-4DD9-A9DF-0DFF6CCCBE72}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>Enterprises by employment size band</t>
   </si>
   <si>
-    <t>Job adverts by profession</t>
-  </si>
-  <si>
     <t>Jan 2021 - Dec 2021 (20/04/22)</t>
   </si>
   <si>
@@ -89,12 +86,6 @@
     <t>Key Stage 5 (KS5) destinations</t>
   </si>
   <si>
-    <t>Dec 2022 (13/02/23)</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/labourdemandvolumesbyprofessionandlocalauthorityukjanuary2017todecember2022'&gt;ONS Textkernel&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Skills Imperative 2035 employment projections by industry, sector, and qualification</t>
   </si>
   <si>
@@ -159,6 +150,15 @@
   </si>
   <si>
     <t>Jan 2023 - Dec 2023 (16/04/24)</t>
+  </si>
+  <si>
+    <t>Job adverts by occupation</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/labourdemandvolumesbystandardoccupationclassificationsoc2020uk'&gt;ONS Textkernel&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>May 2023 (15/03/24)</t>
   </si>
 </sst>
 </file>
@@ -246,9 +246,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -286,7 +286,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -392,7 +392,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -534,7 +534,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -545,7 +545,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -571,30 +571,30 @@
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -605,24 +605,24 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -630,13 +630,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -647,10 +647,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -661,24 +661,24 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -689,49 +689,49 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -739,13 +739,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Update APS refs in DataTable
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/jane8_evans_education_gov_uk/Documents/Documents/Repos/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5CCD392-972B-4DD9-A9DF-0DFF6CCCBE72}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E84A032E-62F9-406A-B13B-7C3F5415CD9E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -131,9 +131,6 @@
     <t>Mar 2024 (Sep 24)</t>
   </si>
   <si>
-    <t>Oct 2022 - Sep 2023 (16/01/24)</t>
-  </si>
-  <si>
     <t>Dec 2021 - Dec 2022 (22/11/23)</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>May 2023 (15/03/24)</t>
+  </si>
+  <si>
+    <t>Apr 2023 - Mar 2024 (18/07/24)</t>
   </si>
 </sst>
 </file>
@@ -243,6 +243,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -545,7 +549,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -577,10 +581,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -591,10 +595,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -605,10 +609,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -619,10 +623,10 @@
         <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -630,13 +634,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -689,10 +693,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
-      </c>
-      <c r="D10" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -725,13 +729,13 @@
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
update quals data to include ncf. add in some caveating around that. add in a level 4 plus metric
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/jane8_evans_education_gov_uk/Documents/Documents/Repos/lsip_dashboard/Data/3-1_DataTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E84A032E-62F9-406A-B13B-7C3F5415CD9E}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9A88C4E-81E0-4BC7-8FFA-2F40739CE296}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>Data​</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Enterprises by employment size band</t>
   </si>
   <si>
-    <t>Jan 2021 - Dec 2021 (20/04/22)</t>
-  </si>
-  <si>
     <t>Key Stage 4 (KS4) destinations</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
   </si>
   <si>
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/further-education-and-skills/2022-23'&gt;Individualised Learner Record&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>TBC depending on ONS recoding the qualification framework.</t>
   </si>
   <si>
     <t>Mar 2023 (27/09/23)</t>
@@ -243,10 +237,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -548,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -575,30 +565,30 @@
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -609,24 +599,24 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -634,13 +624,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -651,10 +641,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -665,24 +655,24 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -693,49 +683,49 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="B13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -743,13 +733,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
         <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
adding in fe achievemnt data , cleaning it and applying to the dahsboard fixing text around that add an aims metric to the dahsboard
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9A88C4E-81E0-4BC7-8FFA-2F40739CE296}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB3E9BD8-66B2-43C4-BC08-72456654E35E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>To be announced</t>
   </si>
   <si>
-    <t>Further education and skills achievements by sector subject area</t>
-  </si>
-  <si>
     <t>Employment by industry</t>
   </si>
   <si>
@@ -92,9 +89,6 @@
     <t>&lt;a href='https://www.gov.uk/government/publications/labour-market-and-skills-projections-2020-to-2035'&gt;Skills Imperative 2035&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Further education and skills achievements and participation by provision, level and age group</t>
-  </si>
-  <si>
     <t>Employment by occupation</t>
   </si>
   <si>
@@ -137,9 +131,6 @@
     <t>Aug 2022 – Jul 2023 (30/11/23)</t>
   </si>
   <si>
-    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/93f9aa79-9a67-48d5-e9e2-08dc0dc60f26'&gt;Individualised Learner Record&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Jan 2023 - Dec 2023 (16/04/24)</t>
   </si>
   <si>
@@ -153,6 +144,15 @@
   </si>
   <si>
     <t>Apr 2023 - Mar 2024 (18/07/24)</t>
+  </si>
+  <si>
+    <t>Further education and skills learner achievements and participation by age group</t>
+  </si>
+  <si>
+    <t>Further education and skills sim achievements by age, sector subject area and level</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/find-statistics/further-education-and-skills'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:D7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -565,167 +565,167 @@
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -733,13 +733,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
         <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Update online job ads data up to Dec 23
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/jane8_evans_education_gov_uk/Documents/Documents/Repos/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9A88C4E-81E0-4BC7-8FFA-2F40739CE296}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1C5AFD6-CD1C-40A0-A2D4-305D8761B91D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -149,10 +149,10 @@
     <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/labourdemandvolumesbystandardoccupationclassificationsoc2020uk'&gt;ONS Textkernel&lt;/a&gt;</t>
   </si>
   <si>
-    <t>May 2023 (15/03/24)</t>
-  </si>
-  <si>
     <t>Apr 2023 - Mar 2024 (18/07/24)</t>
+  </si>
+  <si>
+    <t>Dec 2023 (24/06/24)</t>
   </si>
 </sst>
 </file>
@@ -538,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:D7"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -574,7 +574,7 @@
         <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -588,7 +588,7 @@
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -602,7 +602,7 @@
         <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -644,7 +644,7 @@
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -725,7 +725,7 @@
         <v>36</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
UPdate aps data had to make a fix to get the correct periods for  qualifications data as it was triung to get the latest period but there is no data for that period add in tests to script
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/jane8_evans_education_gov_uk/Documents/Documents/Repos/lsip_dashboard/Data/3-1_DataTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{FDED576E-BB1A-4BAC-8E31-5A3EE1E571AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1C5AFD6-CD1C-40A0-A2D4-305D8761B91D}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="114_{7DF4BC2A-E627-4690-BDAA-C427D3666987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E5C4D5F-C424-4349-A909-A87BD642E578}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>Data​</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>Dec 2023 (24/06/24)</t>
+  </si>
+  <si>
+    <t>Jul 2023 - Jun 2024 (15/10/24)</t>
+  </si>
+  <si>
+    <t>Jan 2024 - Dec 2024 (TBC)</t>
   </si>
 </sst>
 </file>
@@ -539,7 +545,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -571,10 +577,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -585,10 +591,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -599,10 +605,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -644,7 +650,7 @@
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
remove error caveat now that it is fixed keep enterprise error as this is still an error remove the other la errors but note that the as the piblished data will be renamed. howvere we still fix it in the data as we don't have the published data yet, just the original (incorrect) files
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="114_{7DF4BC2A-E627-4690-BDAA-C427D3666987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E5C4D5F-C424-4349-A909-A87BD642E578}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="114_{7DF4BC2A-E627-4690-BDAA-C427D3666987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61964A8F-679C-4994-A743-161B6951DEA2}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -86,9 +86,6 @@
     <t>Skills Imperative 2035 employment projections by industry, sector, and qualification</t>
   </si>
   <si>
-    <t>2035 (16/03/23)</t>
-  </si>
-  <si>
     <t>&lt;a href='https://www.gov.uk/government/publications/labour-market-and-skills-projections-2020-to-2035'&gt;Skills Imperative 2035&lt;/a&gt;</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>Jan 2024 - Dec 2024 (TBC)</t>
+  </si>
+  <si>
+    <t>2035 (02/08/24)</t>
   </si>
 </sst>
 </file>
@@ -544,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -571,30 +571,30 @@
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -605,24 +605,24 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -630,13 +630,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -647,10 +647,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -661,24 +661,24 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -689,10 +689,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
         <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -700,13 +700,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -714,24 +714,24 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
         <v>35</v>
       </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
       <c r="C13" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -742,10 +742,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Following QA from Jane: "*line 949, we should remove 'in the published data' from the error message, because we're not publishing it this time. Instead maybe say 'There is an error in the data for Enterprise M3 LEP (including all of Surrey) LSIP which has prevented it from being included in the published data' Also need to remove 'we are working to get the published data corrected' because we're not. *Publication date for this version will need updating" "*In DataTable  - publication date will need to be updated *In DataText - we will published the alternative scenarios ourselves this time (at UK level) so could change to 'Alternative scenarios are available within the published data for UK only'."
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="114_{7DF4BC2A-E627-4690-BDAA-C427D3666987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61964A8F-679C-4994-A743-161B6951DEA2}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="114_{7DF4BC2A-E627-4690-BDAA-C427D3666987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{108F1FDD-21D5-4026-A47E-15C780369770}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -158,7 +158,7 @@
     <t>Jan 2024 - Dec 2024 (TBC)</t>
   </si>
   <si>
-    <t>2035 (02/08/24)</t>
+    <t>2035 (05/08/24)</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added in latest aps data added in version control added in note on aps accreditation
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\3-1_DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="114_{7DF4BC2A-E627-4690-BDAA-C427D3666987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{108F1FDD-21D5-4026-A47E-15C780369770}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -146,9 +146,6 @@
     <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/labourdemandvolumesbystandardoccupationclassificationsoc2020uk'&gt;ONS Textkernel&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Apr 2023 - Mar 2024 (18/07/24)</t>
-  </si>
-  <si>
     <t>Dec 2023 (24/06/24)</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>2035 (05/08/24)</t>
+  </si>
+  <si>
+    <t>Oct 2023 - Sep 2024 (14/01/25)</t>
   </si>
 </sst>
 </file>
@@ -544,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -577,10 +577,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -591,10 +591,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -605,10 +605,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -650,7 +650,7 @@
         <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -731,7 +731,7 @@
         <v>35</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -745,7 +745,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Update to latest business count data (2024)
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\3-1_DataTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5044B29-5E9B-4AD2-A1C6-319412B93F54}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -104,9 +104,6 @@
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/further-education-and-skills/2022-23'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Mar 2023 (27/09/23)</t>
-  </si>
-  <si>
     <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/f5995891-4e9a-439d-0d58-08dbd1400c33'&gt;National Pupil Database&lt;/a&gt;</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
     <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/b0424f32-b140-44a8-a039-08dbd1466a44'&gt;National Pupil Database&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Mar 2024 (Sep 24)</t>
-  </si>
-  <si>
     <t>Dec 2021 - Dec 2022 (22/11/23)</t>
   </si>
   <si>
@@ -159,6 +153,12 @@
   </si>
   <si>
     <t>Oct 2023 - Sep 2024 (14/01/25)</t>
+  </si>
+  <si>
+    <t>Mar 2024 (17/10/24)</t>
+  </si>
+  <si>
+    <t>Mar 2025 (30/12/25)</t>
   </si>
 </sst>
 </file>
@@ -544,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -577,10 +577,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -591,10 +591,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -605,10 +605,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -619,10 +619,10 @@
         <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -630,13 +630,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -647,10 +647,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -661,10 +661,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -675,10 +675,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -689,10 +689,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -700,13 +700,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -714,24 +714,24 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -745,7 +745,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Update destinations data to ay22/23
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\3-1_DataTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C365DDDE-12B1-4BED-8764-2F0CB143DF24}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -107,18 +107,6 @@
     <t>Mar 2023 (27/09/23)</t>
   </si>
   <si>
-    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/f5995891-4e9a-439d-0d58-08dbd1400c33'&gt;National Pupil Database&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>Aug 2021 -  Jul 2022 (20/21 learners) (19/10/23)</t>
-  </si>
-  <si>
-    <t>Aug 2022 -  Jul 2023 (21/22 learners) (Oct 24)</t>
-  </si>
-  <si>
-    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/b0424f32-b140-44a8-a039-08dbd1466a44'&gt;National Pupil Database&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Mar 2024 (Sep 24)</t>
   </si>
   <si>
@@ -159,6 +147,18 @@
   </si>
   <si>
     <t>Oct 2023 - Sep 2024 (14/01/25)</t>
+  </si>
+  <si>
+    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/86d98c08-f1f2-469f-5a0f-08dcf4c92e7d'&gt;National Pupil Database&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Aug 2022 -  Jul 2023 (21/22 learners) (24/10/24)</t>
+  </si>
+  <si>
+    <t>Aug 2023 -  Jul 2024 (22/23 learners) (Oct 25)</t>
+  </si>
+  <si>
+    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/3c47beb5-97bc-4cb2-5a12-08dcf4c92e7d'&gt;National Pupil Database&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -577,10 +577,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -591,10 +591,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -605,10 +605,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -619,10 +619,10 @@
         <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -630,13 +630,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -647,10 +647,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -664,7 +664,7 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -678,7 +678,7 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -689,10 +689,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -700,13 +700,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -714,24 +714,24 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -745,7 +745,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Update destinations data. Change a few of the caveats around the data
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5044B29-5E9B-4AD2-A1C6-319412B93F54}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E11A2F6A-D266-4C8C-925B-F39B370C4123}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -104,18 +104,6 @@
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/further-education-and-skills/2022-23'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
   <si>
-    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/f5995891-4e9a-439d-0d58-08dbd1400c33'&gt;National Pupil Database&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>Aug 2021 -  Jul 2022 (20/21 learners) (19/10/23)</t>
-  </si>
-  <si>
-    <t>Aug 2022 -  Jul 2023 (21/22 learners) (Oct 24)</t>
-  </si>
-  <si>
-    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/b0424f32-b140-44a8-a039-08dbd1466a44'&gt;National Pupil Database&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Dec 2021 - Dec 2022 (22/11/23)</t>
   </si>
   <si>
@@ -159,6 +147,18 @@
   </si>
   <si>
     <t>Mar 2025 (30/12/25)</t>
+  </si>
+  <si>
+    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/86d98c08-f1f2-469f-5a0f-08dcf4c92e7d'&gt;National Pupil Database&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Aug 2022 -  Jul 2023 (21/22 learners) (24/10/24)</t>
+  </si>
+  <si>
+    <t>Aug 2023 -  Jul 2024 (22/23 learners) (Oct 25)</t>
+  </si>
+  <si>
+    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/3c47beb5-97bc-4cb2-5a12-08dcf4c92e7d'&gt;National Pupil Database&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -577,10 +577,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -591,10 +591,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -605,10 +605,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -619,10 +619,10 @@
         <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -630,13 +630,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -647,10 +647,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -661,10 +661,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -675,10 +675,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -689,10 +689,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -700,13 +700,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -714,24 +714,24 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -745,7 +745,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Update to the latest business demographics data: add new data Read in update text files update version control
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/rory_burke_education_gov_uk/Documents/GiT Projects/Local Skills Dashboard/Local skills dashboard/Data/3-1_DataTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B755C77-28C6-4D4A-BF5B-D2BD455A4847}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D19286B5-3F4B-4288-B2DA-7E02A171184C}"/>
   <bookViews>
-    <workbookView xWindow="-15230" yWindow="10690" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,12 +104,6 @@
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/further-education-and-skills/2022-23'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Dec 2021 - Dec 2022 (22/11/23)</t>
-  </si>
-  <si>
-    <t>Dec 2022 - Dec 2023 (Nov 24)</t>
-  </si>
-  <si>
     <t>Aug 2023 – Jul 2024 (Nov 24)</t>
   </si>
   <si>
@@ -159,6 +153,12 @@
   </si>
   <si>
     <t>Nov 2024 (05/11/24)</t>
+  </si>
+  <si>
+    <t>Dec 2022 - Dec 2023 (18/11/24)</t>
+  </si>
+  <si>
+    <t>Dec 2023 - Dec 2024 (Nov 25)</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -577,10 +577,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -591,10 +591,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -605,10 +605,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -619,10 +619,10 @@
         <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -630,13 +630,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -647,10 +647,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -661,10 +661,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -675,10 +675,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -689,10 +689,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -700,13 +700,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -714,24 +714,24 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -745,7 +745,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Update APS employment data: rerun extract nomis file to bring in new data update data text update version control
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D19286B5-3F4B-4288-B2DA-7E02A171184C}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0AC7B4C-ED78-4CD0-B0BA-01BD6ECFFC90}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -122,18 +122,12 @@
     <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/labourdemandvolumesbystandardoccupationclassificationsoc2020uk'&gt;ONS Textkernel&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Jul 2023 - Jun 2024 (15/10/24)</t>
-  </si>
-  <si>
     <t>Jan 2024 - Dec 2024 (TBC)</t>
   </si>
   <si>
     <t>2035 (05/08/24)</t>
   </si>
   <si>
-    <t>Oct 2023 - Sep 2024 (14/01/25)</t>
-  </si>
-  <si>
     <t>Mar 2024 (17/10/24)</t>
   </si>
   <si>
@@ -159,6 +153,12 @@
   </si>
   <si>
     <t>Dec 2023 - Dec 2024 (Nov 25)</t>
+  </si>
+  <si>
+    <t>Oct 2023 - Sep 2024 (21/01/25)</t>
+  </si>
+  <si>
+    <t>Jan 2024 - Dec 2024 (15/04/25)</t>
   </si>
 </sst>
 </file>
@@ -544,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -577,10 +577,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -591,10 +591,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -605,10 +605,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -650,7 +650,7 @@
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -661,10 +661,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -675,10 +675,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -689,10 +689,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -700,13 +700,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -714,13 +714,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
@@ -731,7 +731,7 @@
         <v>27</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -745,7 +745,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Update ILR data Import latest files Had to make a few changes to some scripts because the column names had changed Update dashboard text Update version
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0AC7B4C-ED78-4CD0-B0BA-01BD6ECFFC90}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2485617A-F658-4672-BC9D-48B8C728E7FB}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -101,18 +101,6 @@
     <t>Enterprises by employment industry</t>
   </si>
   <si>
-    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/further-education-and-skills/2022-23'&gt;Individualised Learner Record&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>Aug 2023 – Jul 2024 (Nov 24)</t>
-  </si>
-  <si>
-    <t>Aug 2022 – Jul 2023 (30/11/23)</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/93f9aa79-9a67-48d5-e9e2-08dc0dc60f26'&gt;Individualised Learner Record&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Jan 2023 - Dec 2023 (16/04/24)</t>
   </si>
   <si>
@@ -159,6 +147,18 @@
   </si>
   <si>
     <t>Jan 2024 - Dec 2024 (15/04/25)</t>
+  </si>
+  <si>
+    <t>Aug 2024 – Jul 2025 (Nov 25)</t>
+  </si>
+  <si>
+    <t>Aug 2023 – Jul 2024 (28/11/24)</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/data-set/b930498d-b4f0-416d-a086-7acee1be8179'&gt;Individualised Learner Record&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/47e8710e-ccb7-401c-ab25-08dd34489990'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -577,10 +577,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -591,10 +591,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -605,10 +605,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -616,13 +616,13 @@
         <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -630,13 +630,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -647,10 +647,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -661,10 +661,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -675,10 +675,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -689,10 +689,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -700,13 +700,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -714,24 +714,24 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -745,7 +745,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Update the online jobs ad data to Nov 2024
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2485617A-F658-4672-BC9D-48B8C728E7FB}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5322E67F-83B8-4BD1-B369-5CA00694E2D7}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -134,9 +134,6 @@
     <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/3c47beb5-97bc-4cb2-5a12-08dcf4c92e7d'&gt;National Pupil Database&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Nov 2024 (05/11/24)</t>
-  </si>
-  <si>
     <t>Dec 2022 - Dec 2023 (18/11/24)</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/47e8710e-ccb7-401c-ab25-08dd34489990'&gt;Individualised Learner Record&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Nov 2024 (07/02/25)</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -577,10 +577,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
         <v>35</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -591,10 +591,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
         <v>35</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -605,10 +605,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
         <v>35</v>
-      </c>
-      <c r="D4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -616,13 +616,13 @@
         <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -630,13 +630,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -689,10 +689,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
         <v>33</v>
-      </c>
-      <c r="D10" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -731,7 +731,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Update destinations data with revised data. The data format had changed a bit so built that into the import file
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5322E67F-83B8-4BD1-B369-5CA00694E2D7}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7FABC4D-C875-4D5D-B00A-A354742858E2}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -122,18 +122,9 @@
     <t>Mar 2025 (30/12/25)</t>
   </si>
   <si>
-    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/86d98c08-f1f2-469f-5a0f-08dcf4c92e7d'&gt;National Pupil Database&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>Aug 2022 -  Jul 2023 (21/22 learners) (24/10/24)</t>
-  </si>
-  <si>
     <t>Aug 2023 -  Jul 2024 (22/23 learners) (Oct 25)</t>
   </si>
   <si>
-    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/3c47beb5-97bc-4cb2-5a12-08dcf4c92e7d'&gt;National Pupil Database&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Dec 2022 - Dec 2023 (18/11/24)</t>
   </si>
   <si>
@@ -159,6 +150,15 @@
   </si>
   <si>
     <t>Nov 2024 (07/02/25)</t>
+  </si>
+  <si>
+    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/find-statistics/16-18-destination-measures'&gt;16-18 destination measures&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/find-statistics/key-stage-4-destination-measures/2022-23'&gt;Key stage 4 destination measures&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Aug 2022 -  Jul 2023 (21/22 learners) (27/02/25)</t>
   </si>
 </sst>
 </file>
@@ -544,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -577,10 +577,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -591,10 +591,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -605,10 +605,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -616,13 +616,13 @@
         <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -630,13 +630,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -689,10 +689,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -700,13 +700,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -714,13 +714,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
@@ -731,7 +731,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Update all the text in the dashboard: the version control, the data sources table, and the footnotes on the job ads page
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7FABC4D-C875-4D5D-B00A-A354742858E2}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B95A015-F28A-46C8-93B5-EF060914017A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -149,9 +149,6 @@
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/47e8710e-ccb7-401c-ab25-08dd34489990'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Nov 2024 (07/02/25)</t>
-  </si>
-  <si>
     <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/find-statistics/16-18-destination-measures'&gt;16-18 destination measures&lt;/a&gt;</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>Aug 2022 -  Jul 2023 (21/22 learners) (27/02/25)</t>
+  </si>
+  <si>
+    <t>Jan 2025 (12/03/25)</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -700,10 +700,10 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>28</v>
@@ -714,10 +714,10 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>28</v>
@@ -731,7 +731,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Update job ads data including some changes as a result of the source data reformating column order and area names
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BA8C8BA-360C-405D-8F2B-F1CD783CB102}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBCCC860-7376-473F-AD63-4E18BE6783BD}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="4360" yWindow="20" windowWidth="15310" windowHeight="14300" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -155,10 +155,10 @@
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/47e8710e-ccb7-401c-ab25-08dd34489990'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Nov 2024 (07/02/25)</t>
-  </si>
-  <si>
     <t>Apr 2024 - Mar 2025 (17/07/25)</t>
+  </si>
+  <si>
+    <t>Feb 2025 (01/04/25)</t>
   </si>
 </sst>
 </file>
@@ -544,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -580,7 +580,7 @@
         <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -594,7 +594,7 @@
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -608,7 +608,7 @@
         <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -731,7 +731,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
A previous merge seems to have failed, so i need to add in a previous data updates manually - the destinations data
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBCCC860-7376-473F-AD63-4E18BE6783BD}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29E94ECA-B4B2-4CBD-9CE1-5CDD3C5D3107}"/>
   <bookViews>
-    <workbookView xWindow="4360" yWindow="20" windowWidth="15310" windowHeight="14300" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -125,9 +125,6 @@
     <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/86d98c08-f1f2-469f-5a0f-08dcf4c92e7d'&gt;National Pupil Database&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Aug 2022 -  Jul 2023 (21/22 learners) (24/10/24)</t>
-  </si>
-  <si>
     <t>Aug 2023 -  Jul 2024 (22/23 learners) (Oct 25)</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>Feb 2025 (01/04/25)</t>
+  </si>
+  <si>
+    <t>Aug 2022 -  Jul 2023 (21/22 learners) (27/02/25)</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -577,10 +577,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -591,10 +591,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -605,10 +605,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -616,13 +616,13 @@
         <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -630,13 +630,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -689,10 +689,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
-      </c>
-      <c r="D10" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -703,10 +703,10 @@
         <v>28</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -714,13 +714,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
@@ -731,7 +731,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Correct destination links Update version control date
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29E94ECA-B4B2-4CBD-9CE1-5CDD3C5D3107}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7347B5D-8E7A-4617-A10E-CE3C30D2684D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -122,15 +122,9 @@
     <t>Mar 2025 (30/12/25)</t>
   </si>
   <si>
-    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/86d98c08-f1f2-469f-5a0f-08dcf4c92e7d'&gt;National Pupil Database&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Aug 2023 -  Jul 2024 (22/23 learners) (Oct 25)</t>
   </si>
   <si>
-    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/3c47beb5-97bc-4cb2-5a12-08dcf4c92e7d'&gt;National Pupil Database&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Dec 2022 - Dec 2023 (18/11/24)</t>
   </si>
   <si>
@@ -159,6 +153,12 @@
   </si>
   <si>
     <t>Aug 2022 -  Jul 2023 (21/22 learners) (27/02/25)</t>
+  </si>
+  <si>
+    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/find-statistics/key-stage-4-destination-measures/2022-23'&gt;Key stage 4 destination measures&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/find-statistics/16-18-destination-measures/2022-23'&gt;16-18 destination measures&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -577,10 +577,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -591,10 +591,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -605,10 +605,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -616,13 +616,13 @@
         <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -630,13 +630,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -689,10 +689,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -700,13 +700,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -714,13 +714,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
@@ -731,7 +731,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Update to latest job ad data Update data text and sources Update version control
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7347B5D-8E7A-4617-A10E-CE3C30D2684D}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4994510D-CABC-4A91-9F4C-E12CD12C6015}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="15310" windowHeight="14300" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>Data​</t>
   </si>
@@ -149,9 +149,6 @@
     <t>Apr 2024 - Mar 2025 (17/07/25)</t>
   </si>
   <si>
-    <t>Feb 2025 (01/04/25)</t>
-  </si>
-  <si>
     <t>Aug 2022 -  Jul 2023 (21/22 learners) (27/02/25)</t>
   </si>
   <si>
@@ -159,6 +156,12 @@
   </si>
   <si>
     <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/find-statistics/16-18-destination-measures/2022-23'&gt;16-18 destination measures&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Mar 2025 (25/04/25)</t>
+  </si>
+  <si>
+    <t>Apr 2025 (May 2025)</t>
   </si>
 </sst>
 </file>
@@ -544,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -700,10 +703,10 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>28</v>
@@ -714,10 +717,10 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>28</v>
@@ -731,10 +734,10 @@
         <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update qualification data Update data text and data sources text Update version control
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4994510D-CABC-4A91-9F4C-E12CD12C6015}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B115D165-CF51-4A2C-8964-8F5DC519E60F}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="15310" windowHeight="14300" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>Data​</t>
   </si>
@@ -101,18 +101,12 @@
     <t>Enterprises by employment industry</t>
   </si>
   <si>
-    <t>Jan 2023 - Dec 2023 (16/04/24)</t>
-  </si>
-  <si>
     <t>Job adverts by occupation</t>
   </si>
   <si>
     <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/labourdemandvolumesbystandardoccupationclassificationsoc2020uk'&gt;ONS Textkernel&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Jan 2024 - Dec 2024 (TBC)</t>
-  </si>
-  <si>
     <t>2035 (05/08/24)</t>
   </si>
   <si>
@@ -162,6 +156,9 @@
   </si>
   <si>
     <t>Apr 2025 (May 2025)</t>
+  </si>
+  <si>
+    <t>Jan 2025 - Dec 2025 (Apr 26)</t>
   </si>
 </sst>
 </file>
@@ -547,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -580,10 +577,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -594,10 +591,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -608,10 +605,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -619,13 +616,13 @@
         <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -633,13 +630,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -650,10 +647,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -664,10 +661,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -678,10 +675,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -692,10 +689,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -703,13 +700,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -717,27 +714,27 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
       <c r="C13" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -748,7 +745,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Update job ads data. The format of the raw data changed to exclude 2 digit SOC and to exclude summaries at LEP, LSIP and MCA levels. Therefore values were calculated from 3 digit soc and from LAD level data.
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B115D165-CF51-4A2C-8964-8F5DC519E60F}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4509007-0730-4BF6-B8FD-E851F09F0168}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -152,13 +152,13 @@
     <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/find-statistics/16-18-destination-measures/2022-23'&gt;16-18 destination measures&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Mar 2025 (25/04/25)</t>
-  </si>
-  <si>
-    <t>Apr 2025 (May 2025)</t>
-  </si>
-  <si>
     <t>Jan 2025 - Dec 2025 (Apr 26)</t>
+  </si>
+  <si>
+    <t>May 2025 (26/06/25)</t>
+  </si>
+  <si>
+    <t>Jun 2025 (Jul 2025)</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -650,7 +650,7 @@
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -731,10 +731,10 @@
         <v>22</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update to latest APS data Update data sources and text tables Run tests
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4509007-0730-4BF6-B8FD-E851F09F0168}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F3D9AD3-255B-4F1D-878E-44FCBABAACD7}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>Data​</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>Jun 2025 (Jul 2025)</t>
+  </si>
+  <si>
+    <t>Jul 2024 - Jun 2025 (14/10/25)</t>
   </si>
 </sst>
 </file>
@@ -544,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -577,10 +580,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -591,10 +594,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -605,10 +608,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update online job ads data to June 2025 data
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F3D9AD3-255B-4F1D-878E-44FCBABAACD7}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCDB3196-C2D7-4356-A302-442DB89EFE01}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -155,13 +155,13 @@
     <t>Jan 2025 - Dec 2025 (Apr 26)</t>
   </si>
   <si>
-    <t>May 2025 (26/06/25)</t>
-  </si>
-  <si>
-    <t>Jun 2025 (Jul 2025)</t>
-  </si>
-  <si>
     <t>Jul 2024 - Jun 2025 (14/10/25)</t>
+  </si>
+  <si>
+    <t>Jul 2025 (29/08/25)</t>
+  </si>
+  <si>
+    <t>Jun 2025 (01/08/25)</t>
   </si>
 </sst>
 </file>
@@ -548,7 +548,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -583,7 +583,7 @@
         <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -597,7 +597,7 @@
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -611,7 +611,7 @@
         <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -734,7 +734,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Update online job ads data to July 2025 data
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmt1pr-dhfs01\Personal\MMEHTA4\Repos\lsip_dashboard\Data\3-1_DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{B1C53E57-9A20-4D3A-B86C-D2FC386A6F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCDB3196-C2D7-4356-A302-442DB89EFE01}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E491BE-4718-4455-9A42-DB20A1EB32F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -161,14 +161,14 @@
     <t>Jul 2025 (29/08/25)</t>
   </si>
   <si>
-    <t>Jun 2025 (01/08/25)</t>
+    <t>Aug 2025 (September (TBC))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,12 +196,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FF323132"/>
-      <name val="Open Sans"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -223,14 +217,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,9 +540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -733,11 +724,11 @@
       <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
         <v>41</v>
-      </c>
-      <c r="D13" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Ast the nomis api to account for the new naming of MCA grouping. Adjust within import code as well. Temporarily filter out the new MCAs (to be used across the dashboard at a future date). Correct data source text
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmt1pr-dhfs01\Personal\MMEHTA4\Repos\lsip_dashboard\Data\3-1_DataTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E491BE-4718-4455-9A42-DB20A1EB32F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{49E491BE-4718-4455-9A42-DB20A1EB32F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C781C487-00E3-4793-BEA9-5992C48305CE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="6740" yWindow="20" windowWidth="15310" windowHeight="14300" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -161,7 +161,7 @@
     <t>Jul 2025 (29/08/25)</t>
   </si>
   <si>
-    <t>Aug 2025 (September (TBC))</t>
+    <t>Aug 2025 (Sep 25)</t>
   </si>
 </sst>
 </file>
@@ -540,7 +540,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
Add in some navigation buttons. Clean up CSS code. Add in job ads note.
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\3-1_DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{49E491BE-4718-4455-9A42-DB20A1EB32F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C781C487-00E3-4793-BEA9-5992C48305CE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01EFA5B-317B-479C-99B8-943AF476D39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6740" yWindow="20" windowWidth="15310" windowHeight="14300" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -161,7 +161,7 @@
     <t>Jul 2025 (29/08/25)</t>
   </si>
   <si>
-    <t>Aug 2025 (Sep 25)</t>
+    <t>Sep 2025 (Oct 25)*</t>
   </si>
 </sst>
 </file>
@@ -540,7 +540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update to the latest Business count data.
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\3-1_DataTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01EFA5B-317B-479C-99B8-943AF476D39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{E01EFA5B-317B-479C-99B8-943AF476D39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FE3080C-3449-4CBC-85EB-7F4DACBE8252}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -110,12 +110,6 @@
     <t>2035 (05/08/24)</t>
   </si>
   <si>
-    <t>Mar 2024 (17/10/24)</t>
-  </si>
-  <si>
-    <t>Mar 2025 (30/12/25)</t>
-  </si>
-  <si>
     <t>Aug 2023 -  Jul 2024 (22/23 learners) (Oct 25)</t>
   </si>
   <si>
@@ -162,6 +156,12 @@
   </si>
   <si>
     <t>Sep 2025 (Oct 25)*</t>
+  </si>
+  <si>
+    <t>Mar 2025 (14/10/24)</t>
+  </si>
+  <si>
+    <t>Mar 2026 (Autumn 26)</t>
   </si>
 </sst>
 </file>
@@ -541,7 +541,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -573,10 +573,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -587,10 +587,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -601,10 +601,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -612,13 +612,13 @@
         <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -626,13 +626,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -643,10 +643,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -657,10 +657,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -671,10 +671,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -685,10 +685,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -696,13 +696,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -710,13 +710,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
@@ -727,10 +727,10 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update the destinations data to the latest.
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{E01EFA5B-317B-479C-99B8-943AF476D39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FE3080C-3449-4CBC-85EB-7F4DACBE8252}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{E01EFA5B-317B-479C-99B8-943AF476D39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57F6C660-192F-4299-A730-A6C03556DD6D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -110,9 +110,6 @@
     <t>2035 (05/08/24)</t>
   </si>
   <si>
-    <t>Aug 2023 -  Jul 2024 (22/23 learners) (Oct 25)</t>
-  </si>
-  <si>
     <t>Dec 2022 - Dec 2023 (18/11/24)</t>
   </si>
   <si>
@@ -137,15 +134,6 @@
     <t>Apr 2024 - Mar 2025 (17/07/25)</t>
   </si>
   <si>
-    <t>Aug 2022 -  Jul 2023 (21/22 learners) (27/02/25)</t>
-  </si>
-  <si>
-    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/find-statistics/key-stage-4-destination-measures/2022-23'&gt;Key stage 4 destination measures&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/find-statistics/16-18-destination-measures/2022-23'&gt;16-18 destination measures&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Jan 2025 - Dec 2025 (Apr 26)</t>
   </si>
   <si>
@@ -162,6 +150,18 @@
   </si>
   <si>
     <t>Mar 2026 (Autumn 26)</t>
+  </si>
+  <si>
+    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/find-statistics/16-18-destination-measures'&gt;16-18 destination measures&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/find-statistics/key-stage-4-destination-measures/'&gt;Key stage 4 destination measures&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Aug 2023 -  Jul 2024 (22/23 learners) (16/10/25)</t>
+  </si>
+  <si>
+    <t>Aug 2023 -  Jul 2024 (22/23 learners) (Feb 26)</t>
   </si>
 </sst>
 </file>
@@ -541,7 +541,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -573,10 +573,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -587,10 +587,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -601,10 +601,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -612,13 +612,13 @@
         <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -626,13 +626,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -643,10 +643,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -657,10 +657,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -671,10 +671,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -685,10 +685,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
         <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -696,13 +696,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -710,13 +710,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
@@ -727,10 +727,10 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update data text for the destinations data years. Update data table for the new APS data.
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-1_DataTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\3-1_DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{E01EFA5B-317B-479C-99B8-943AF476D39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57F6C660-192F-4299-A730-A6C03556DD6D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3528C90A-B688-47B8-A04C-1AE289EAAB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -131,9 +131,6 @@
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/47e8710e-ccb7-401c-ab25-08dd34489990'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Apr 2024 - Mar 2025 (17/07/25)</t>
-  </si>
-  <si>
     <t>Jan 2025 - Dec 2025 (Apr 26)</t>
   </si>
   <si>
@@ -162,6 +159,9 @@
   </si>
   <si>
     <t>Aug 2023 -  Jul 2024 (22/23 learners) (Feb 26)</t>
+  </si>
+  <si>
+    <t>Oct 2024 - Sep 2025 (20/01/26)</t>
   </si>
 </sst>
 </file>
@@ -541,7 +541,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -573,10 +573,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -587,10 +587,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -601,10 +601,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -646,7 +646,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -657,10 +657,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
         <v>36</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -671,10 +671,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
         <v>36</v>
-      </c>
-      <c r="D9" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -696,13 +696,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -710,13 +710,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
@@ -727,10 +727,10 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
         <v>34</v>
-      </c>
-      <c r="D13" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update job ads data sources and note.
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\3-1_DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3528C90A-B688-47B8-A04C-1AE289EAAB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C1AC85-9D6F-4240-8084-FEF026870769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -140,9 +140,6 @@
     <t>Jul 2025 (29/08/25)</t>
   </si>
   <si>
-    <t>Sep 2025 (Oct 25)*</t>
-  </si>
-  <si>
     <t>Mar 2025 (14/10/24)</t>
   </si>
   <si>
@@ -162,6 +159,9 @@
   </si>
   <si>
     <t>Oct 2024 - Sep 2025 (20/01/26)</t>
+  </si>
+  <si>
+    <t>TBC*</t>
   </si>
 </sst>
 </file>
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -576,7 +576,7 @@
         <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -590,7 +590,7 @@
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -604,7 +604,7 @@
         <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -657,10 +657,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
         <v>35</v>
-      </c>
-      <c r="D8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -671,10 +671,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
         <v>35</v>
-      </c>
-      <c r="D9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -696,13 +696,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -710,13 +710,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
@@ -730,7 +730,7 @@
         <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update to business demography 2025 release
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\3-1_DataTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jevans8\Repos\lsip_dashboard\Data\3-1_DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C1AC85-9D6F-4240-8084-FEF026870769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75EA214-51D1-46BB-A7DD-7736441E53E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -110,12 +110,6 @@
     <t>2035 (05/08/24)</t>
   </si>
   <si>
-    <t>Dec 2022 - Dec 2023 (18/11/24)</t>
-  </si>
-  <si>
-    <t>Dec 2023 - Dec 2024 (Nov 25)</t>
-  </si>
-  <si>
     <t>Jan 2024 - Dec 2024 (15/04/25)</t>
   </si>
   <si>
@@ -162,6 +156,12 @@
   </si>
   <si>
     <t>TBC*</t>
+  </si>
+  <si>
+    <t>Dec 2023 - Dec 2024 (20/11/25)</t>
+  </si>
+  <si>
+    <t>Dec 2024 - Dec 2025 (Nov 26)</t>
   </si>
 </sst>
 </file>
@@ -541,7 +541,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -573,10 +573,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -587,10 +587,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -601,10 +601,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -612,13 +612,13 @@
         <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -626,13 +626,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -643,10 +643,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -657,10 +657,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -671,10 +671,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -685,10 +685,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -696,13 +696,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -710,13 +710,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
@@ -727,10 +727,10 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update input files to 2025 FE data
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/DataTable.xlsx
+++ b/Data/3-1_DataTable/DataTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jevans8\Repos\lsip_dashboard\Data\3-1_DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75EA214-51D1-46BB-A7DD-7736441E53E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91CA5E8E-A54C-4860-B017-C7DC9575D383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -113,18 +113,6 @@
     <t>Jan 2024 - Dec 2024 (15/04/25)</t>
   </si>
   <si>
-    <t>Aug 2024 – Jul 2025 (Nov 25)</t>
-  </si>
-  <si>
-    <t>Aug 2023 – Jul 2024 (28/11/24)</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/data-set/b930498d-b4f0-416d-a086-7acee1be8179'&gt;Individualised Learner Record&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/47e8710e-ccb7-401c-ab25-08dd34489990'&gt;Individualised Learner Record&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Jan 2025 - Dec 2025 (Apr 26)</t>
   </si>
   <si>
@@ -162,6 +150,18 @@
   </si>
   <si>
     <t>Dec 2024 - Dec 2025 (Nov 26)</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/data-set/1977cdbc-7eae-4257-a8c9-3281bb2dbfa9'&gt;Individualised Learner Record&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/529ad7b1-7a0f-419c-eb81-08de29d3af56'&gt;Individualised Learner Record&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Aug 2024 – Jul 2025 (27/11/25)</t>
+  </si>
+  <si>
+    <t>Aug 2025 – Jul 2026 (Nov 26)</t>
   </si>
 </sst>
 </file>
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -573,10 +573,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -587,10 +587,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -601,10 +601,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -612,13 +612,13 @@
         <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -626,13 +626,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -646,7 +646,7 @@
         <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -657,10 +657,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -671,10 +671,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -685,10 +685,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -696,13 +696,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -710,13 +710,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
@@ -727,10 +727,10 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>